<commit_message>
v4-5 upgrade: add ThorlabsSM2L30-XT66P2M_H94mm(axis2base)
Update v4-5-upgrade-parts-list.xlsx
</commit_message>
<xml_diff>
--- a/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
+++ b/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\v4-5-upgrade-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\GitHub-public\benchtop-hardware\v4-5-upgrade-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2769D6-EDEB-404C-A613-AF9A919C2BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7188" yWindow="7704" windowWidth="34560" windowHeight="15864" xr2:uid="{41B90232-ADE7-4C34-A1C8-F3E59EA1C38C}"/>
+    <workbookView xWindow="7188" yWindow="7704" windowWidth="34560" windowHeight="15864"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -261,13 +260,34 @@
   </si>
   <si>
     <t>Machined from Alu, requires SM2 threads</t>
+  </si>
+  <si>
+    <t>ThorlabsSM2L30-XT66P2M_H94mm(axis2base)</t>
+  </si>
+  <si>
+    <t>Rail carriage mount of the SM2 tube assembly</t>
+  </si>
+  <si>
+    <t>Bolted to the Newport CXL95 rail carriages (M6 bolts)</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>Camera-specific support structure</t>
+  </si>
+  <si>
+    <t>Supports the weight of the camera</t>
+  </si>
+  <si>
+    <t>Total, EUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +398,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -454,7 +481,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -479,10 +506,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Heading 1" xfId="1" xr:uid="{EE47BA37-90CF-4BCE-BA68-97355374E575}"/>
-    <cellStyle name="Excel Built-in Note" xfId="2" xr:uid="{56F6E422-8DF4-403D-97F2-4BE2541F67CC}"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="1"/>
+    <cellStyle name="Excel Built-in Note" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -795,11 +824,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65F4918-000C-4ED8-8AF5-E08B4DB93BB3}">
-  <dimension ref="A1:H32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1371,11 +1400,68 @@
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
     </row>
+    <row r="33" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="24">
+        <v>2</v>
+      </c>
+      <c r="E33" s="24">
+        <v>5</v>
+      </c>
+      <c r="F33" s="24">
+        <f>D33*E33</f>
+        <v>10</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="15">
+        <v>1</v>
+      </c>
+      <c r="E34" s="15">
+        <v>50</v>
+      </c>
+      <c r="F34" s="15">
+        <f>D34*E34</f>
+        <v>50</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="25">
+        <f>SUM(F4:F39)</f>
+        <v>26162</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" xr:uid="{333C5FCF-E80B-4370-A613-1A7440E4B2D7}"/>
-    <hyperlink ref="C24" r:id="rId2" xr:uid="{6D6B149E-6EF0-44E1-AF5A-49FB8DAE6504}"/>
-    <hyperlink ref="C26" r:id="rId3" display="MT-1 Accessory Tube Lens" xr:uid="{63F3362D-4D89-4503-83EA-B83A838A8B48}"/>
+    <hyperlink ref="C8" r:id="rId1"/>
+    <hyperlink ref="C24" r:id="rId2"/>
+    <hyperlink ref="C26" r:id="rId3" display="MT-1 Accessory Tube Lens"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
update v4-5 upgrade parts list
</commit_message>
<xml_diff>
--- a/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
+++ b/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\v4-5-upgrade-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F85063-FE47-4B32-8298-7ED7142A2B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E380F-0508-4973-9897-778BE9D33817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7284" yWindow="6840" windowWidth="34560" windowHeight="15864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -116,9 +116,6 @@
     <t>Adapters for both sides of the ZWO EFW Mini filter, which has T-mount threads (M42)</t>
   </si>
   <si>
-    <t>SM2 coupler to rotate the filter wheel and fix it at desired angle the with retaining ring</t>
-  </si>
-  <si>
     <t>3D printed (SLS)</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>Preferred choice for Mititoyo objectives, except the 2X/0.055 one. Ordered from Edmund for historical reasons, update part number to Mitutoyo</t>
   </si>
   <si>
-    <t>Detection Assembly Mounting (on the rail carriage)</t>
-  </si>
-  <si>
     <t>Detection: Tube lens and camera F-mount</t>
   </si>
   <si>
@@ -266,15 +260,9 @@
     <t>Bolted to the Newport CXL95 rail carriages (M6 bolts)</t>
   </si>
   <si>
-    <t>todo</t>
-  </si>
-  <si>
     <t>Camera-specific support structure</t>
   </si>
   <si>
-    <t>Supports the weight of the camera</t>
-  </si>
-  <si>
     <t>Unit Price (USD)</t>
   </si>
   <si>
@@ -282,6 +270,48 @@
   </si>
   <si>
     <t>Total, USD</t>
+  </si>
+  <si>
+    <t>SM2V05</t>
+  </si>
+  <si>
+    <t>Ø2" Adjustable Lens Tube, 0.31" Travel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM2 coupler to rotate the turret relative to filter wheel </t>
+  </si>
+  <si>
+    <t>SM2 coupler to rotate the F mount (camera) relative to filter wheel</t>
+  </si>
+  <si>
+    <t>XT95-500</t>
+  </si>
+  <si>
+    <t>95 mm Construction Rail, Clear Anodized, L = 500 mm</t>
+  </si>
+  <si>
+    <t>XT95P3</t>
+  </si>
+  <si>
+    <t>Base Plate for 95 mm Rails</t>
+  </si>
+  <si>
+    <t>XT95RC4/M</t>
+  </si>
+  <si>
+    <t>Drop-On Rail Carriage for 95 mm Rails, 100.0 mm Long, M6 Tapped Holes</t>
+  </si>
+  <si>
+    <t>Gantry elements, ONLY for mesoSPIM-v4 upgrade</t>
+  </si>
+  <si>
+    <t>Photometrics Iris 15: ToDo. Orca Lightning: Breadboard 200 mm wide that supports the weight of the camera</t>
+  </si>
+  <si>
+    <t>camera-dependent</t>
+  </si>
+  <si>
+    <t>Detection Assembly Mounting (on the X95 rail carriage)</t>
   </si>
 </sst>
 </file>
@@ -416,12 +446,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -439,6 +463,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -478,19 +508,13 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -500,25 +524,31 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Heading 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -836,643 +866,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="46.77734375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="15"/>
-    <col min="5" max="5" width="20.88671875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="15" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="1" width="39.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="46.77734375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="9"/>
+    <col min="5" max="5" width="20.88671875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="32" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
         <v>12350</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="19">
         <f>E4*D4</f>
         <v>12350</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="27"/>
-    </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="27"/>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
         <v>200</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="19">
         <f>E8*D8</f>
         <v>200</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="3">
         <v>5</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="4">
         <v>10</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="20">
         <f>E9*D9</f>
         <v>50</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
         <v>37</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="19">
         <f>E10*D10</f>
         <v>37</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>49</v>
+      </c>
+      <c r="F11" s="19">
+        <f>E11*D11</f>
+        <v>49</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>24</v>
+      </c>
+      <c r="F12" s="19">
+        <f>E12*D12</f>
+        <v>48</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+    </row>
+    <row r="16" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>4655</v>
+      </c>
+      <c r="F16" s="21">
+        <f>D16*E16</f>
+        <v>4655</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10">
+        <v>75</v>
+      </c>
+      <c r="F17" s="22">
+        <f>D17*E17</f>
+        <v>75</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10">
+        <v>136</v>
+      </c>
+      <c r="F18" s="22">
+        <f>D18*E18</f>
+        <v>136</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
+        <v>100</v>
+      </c>
+      <c r="F19" s="23">
+        <f>D19*E19</f>
+        <v>100</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="5">
-        <v>24</v>
-      </c>
-      <c r="F11" s="26">
-        <f>E11*D11</f>
-        <v>48</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="27"/>
-    </row>
-    <row r="15" spans="1:8" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1</v>
-      </c>
-      <c r="E15" s="14">
-        <v>4655</v>
-      </c>
-      <c r="F15" s="29">
-        <f>D15*E15</f>
-        <v>4655</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16">
-        <v>75</v>
-      </c>
-      <c r="F16" s="30">
-        <f>D16*E16</f>
-        <v>75</v>
-      </c>
-      <c r="G16" s="16" t="s">
+      <c r="F20" s="19">
+        <f>E20*D20</f>
+        <v>26</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="16" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="16">
-        <v>136</v>
-      </c>
-      <c r="F17" s="30">
-        <f>D17*E17</f>
-        <v>136</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="22">
-        <v>1</v>
-      </c>
-      <c r="E18" s="22">
-        <v>100</v>
-      </c>
-      <c r="F18" s="31">
-        <f>D18*E18</f>
-        <v>100</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5">
-        <v>26</v>
-      </c>
-      <c r="F19" s="26">
-        <f>E19*D19</f>
-        <v>26</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="B21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="D21" s="11">
+        <v>1</v>
+      </c>
+      <c r="E21" s="11">
+        <v>801</v>
+      </c>
+      <c r="F21" s="24">
+        <f>D21*E21</f>
+        <v>801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="17">
-        <v>1</v>
-      </c>
-      <c r="E20" s="17">
-        <v>801</v>
-      </c>
-      <c r="F20" s="32">
-        <f>D20*E20</f>
-        <v>801</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="B22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="D22" s="11">
+        <v>1</v>
+      </c>
+      <c r="E22" s="11">
+        <v>718</v>
+      </c>
+      <c r="F22" s="24">
+        <f t="shared" ref="F22:F25" si="0">D22*E22</f>
+        <v>718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="17">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17">
-        <v>718</v>
-      </c>
-      <c r="F21" s="32">
-        <f t="shared" ref="F21:F24" si="0">D21*E21</f>
-        <v>718</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="B23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="17">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17">
+      <c r="D23" s="11">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11">
         <v>1391</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F23" s="24">
         <f t="shared" si="0"/>
         <v>1391</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+    <row r="24" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="17">
-        <v>1</v>
-      </c>
-      <c r="E23" s="17">
+      <c r="D24" s="11">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11">
         <v>883</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F24" s="24">
         <f t="shared" si="0"/>
         <v>883</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="C25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
         <v>3670</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F25" s="24">
         <f t="shared" si="0"/>
         <v>3670</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="19" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="33"/>
-    </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="C27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>752</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" ref="F27:F31" si="1">D27*E27</f>
+        <v>752</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5">
-        <v>752</v>
-      </c>
-      <c r="F26" s="26">
-        <f t="shared" ref="F26:F30" si="1">D26*E26</f>
-        <v>752</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+      <c r="B28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="9">
-        <v>1</v>
-      </c>
-      <c r="E27" s="10">
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4">
         <v>10</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F28" s="20">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
         <v>65</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F29" s="19">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G29" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="B30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5">
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
         <v>32</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F30" s="19">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="B31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="4">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5">
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
         <v>112</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F31" s="19">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="19" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="33"/>
-    </row>
-    <row r="33" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="G31" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="17">
+        <v>2</v>
+      </c>
+      <c r="E34" s="17">
+        <v>10</v>
+      </c>
+      <c r="F34" s="26">
+        <f>D34*E34</f>
+        <v>20</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="23" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="9">
+        <v>3</v>
+      </c>
+      <c r="E35" s="9">
+        <v>150</v>
+      </c>
+      <c r="F35" s="18">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="9">
+        <v>2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>53</v>
+      </c>
+      <c r="F36" s="18">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="9">
+        <v>3</v>
+      </c>
+      <c r="E37" s="9">
+        <v>128</v>
+      </c>
+      <c r="F37" s="18">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="23">
-        <v>2</v>
-      </c>
-      <c r="E33" s="23">
-        <v>10</v>
-      </c>
-      <c r="F33" s="34">
-        <f>D33*E33</f>
-        <v>20</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="D38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <v>50</v>
+      </c>
+      <c r="F38" s="18">
+        <f>D38*E38</f>
+        <v>50</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E45" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="15">
-        <v>1</v>
-      </c>
-      <c r="E34" s="15">
-        <v>50</v>
-      </c>
-      <c r="F34" s="24">
-        <f>D34*E34</f>
-        <v>50</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E41" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="36">
-        <f>SUM(F4:F39)</f>
-        <v>26181</v>
+      <c r="F45" s="28">
+        <f>SUM(F4:F43)</f>
+        <v>26230</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C26" r:id="rId3" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C25" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C27" r:id="rId3" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
add safety rail carriages
</commit_message>
<xml_diff>
--- a/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
+++ b/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\v4-5-upgrade-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E380F-0508-4973-9897-778BE9D33817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFDB0CD-29ED-4231-ADC7-CC4B5BABA48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -312,13 +312,19 @@
   </si>
   <si>
     <t>Detection Assembly Mounting (on the X95 rail carriage)</t>
+  </si>
+  <si>
+    <t>XT95RC1/M</t>
+  </si>
+  <si>
+    <t>Drop-On Rail Carriage for 95 mm Rails, 25.0 mm Long, M6 Tapped Holes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +441,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -511,7 +524,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -549,6 +562,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Heading 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -866,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1489,105 +1504,128 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="37">
         <v>3</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="37">
         <v>150</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="38">
         <v>0</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="37">
         <v>2</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="37">
         <v>53</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="38">
         <v>0</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="37">
         <v>3</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="37">
         <v>128</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F37" s="38">
         <v>0</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+    <row r="38" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="37">
+        <v>2</v>
+      </c>
+      <c r="E38" s="37">
+        <v>77</v>
+      </c>
+      <c r="F38" s="38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="9">
-        <v>1</v>
-      </c>
-      <c r="E38" s="9">
+      <c r="D39" s="9">
+        <v>1</v>
+      </c>
+      <c r="E39" s="9">
         <v>50</v>
       </c>
-      <c r="F38" s="18">
-        <f>D38*E38</f>
+      <c r="F39" s="18">
+        <f>D39*E39</f>
         <v>50</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E45" s="27" t="s">
+    <row r="46" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E46" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="F45" s="28">
-        <f>SUM(F4:F43)</f>
+      <c r="F46" s="28">
+        <f>SUM(F4:F44)</f>
         <v>26230</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upload alignment target file
</commit_message>
<xml_diff>
--- a/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
+++ b/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\v4-5-upgrade-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFDB0CD-29ED-4231-ADC7-CC4B5BABA48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3088CEE9-6AA5-4115-81B6-F5C1711BC878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5376" yWindow="5160" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,15 +272,6 @@
     <t>Total, USD</t>
   </si>
   <si>
-    <t>SM2V05</t>
-  </si>
-  <si>
-    <t>Ø2" Adjustable Lens Tube, 0.31" Travel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SM2 coupler to rotate the turret relative to filter wheel </t>
-  </si>
-  <si>
     <t>SM2 coupler to rotate the F mount (camera) relative to filter wheel</t>
   </si>
   <si>
@@ -318,6 +309,15 @@
   </si>
   <si>
     <t>Drop-On Rail Carriage for 95 mm Rails, 25.0 mm Long, M6 Tapped Holes</t>
+  </si>
+  <si>
+    <t>SM2V10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM2 coupler to mount and rotate the turret relative to filter wheel </t>
+  </si>
+  <si>
+    <t>Ø2" Adjustable Lens Tube, 0.81" Travel</t>
   </si>
 </sst>
 </file>
@@ -884,7 +884,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1059,31 +1059,31 @@
         <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F11" s="19">
         <f>E11*D11</f>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
     </row>
     <row r="33" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="25"/>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="35" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D35" s="37">
         <v>3</v>
@@ -1524,18 +1524,18 @@
         <v>0</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B36" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D36" s="37">
         <v>2</v>
@@ -1547,18 +1547,18 @@
         <v>0</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D37" s="37">
         <v>3</v>
@@ -1570,18 +1570,18 @@
         <v>0</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B38" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D38" s="37">
         <v>2</v>
@@ -1593,15 +1593,15 @@
         <v>0</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>74</v>
@@ -1617,7 +1617,7 @@
         <v>50</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="F46" s="28">
         <f>SUM(F4:F44)</f>
-        <v>26230</v>
+        <v>26235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change filter wheel to ZWO 7x36mm
</commit_message>
<xml_diff>
--- a/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
+++ b/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\v4-5-upgrade-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3088CEE9-6AA5-4115-81B6-F5C1711BC878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91A1199-0A66-4DCC-9FE0-9C35FA716CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="5160" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -74,30 +74,15 @@
     <t>5-slot filter wheel for 25-mm filters</t>
   </si>
   <si>
-    <t>ZWO EFW-MINI</t>
-  </si>
-  <si>
     <t>ZWO</t>
   </si>
   <si>
-    <t xml:space="preserve">ZWO EFW Mini 5 x 31 mm </t>
-  </si>
-  <si>
     <t>Check local distributors (astronomy shops)</t>
   </si>
   <si>
-    <t>25mmFilterAdapter.stl</t>
-  </si>
-  <si>
     <t>3D printed</t>
   </si>
   <si>
-    <t>Adapter to hold 25 mm filters in 31 mm slots</t>
-  </si>
-  <si>
-    <t>See /custom-parts/detection-accessories for printable 3D model</t>
-  </si>
-  <si>
     <t>Thorlabs</t>
   </si>
   <si>
@@ -318,6 +303,18 @@
   </si>
   <si>
     <t>Ø2" Adjustable Lens Tube, 0.81" Travel</t>
+  </si>
+  <si>
+    <t>ZWO EFW 7x36mm</t>
+  </si>
+  <si>
+    <t>32mmFilterAdapter.stl</t>
+  </si>
+  <si>
+    <t>TODO for 32 mm filter in 36 mm slots (available 25mm filter for 31 mm slots). See /custom-parts/detection-accessories for printable 3D model</t>
+  </si>
+  <si>
+    <t>Adapter to hold 32 mm filters in 36 mm slots</t>
   </si>
 </sst>
 </file>
@@ -524,7 +521,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -564,6 +561,7 @@
     <xf numFmtId="1" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Heading 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -884,7 +882,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -913,10 +911,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>4</v>
@@ -991,38 +989,38 @@
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>200</v>
+        <v>299</v>
       </c>
       <c r="F8" s="19">
         <f>E8*D8</f>
-        <v>200</v>
+        <v>299</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3">
         <v>5</v>
@@ -1035,18 +1033,18 @@
         <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1059,18 +1057,18 @@
         <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1083,18 +1081,18 @@
         <v>54</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -1107,32 +1105,32 @@
         <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:8" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
@@ -1145,18 +1143,18 @@
         <v>4655</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
@@ -1169,18 +1167,18 @@
         <v>75</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
@@ -1193,18 +1191,18 @@
         <v>136</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D19" s="16">
         <v>1</v>
@@ -1217,18 +1215,18 @@
         <v>100</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1241,18 +1239,18 @@
         <v>26</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D21" s="11">
         <v>1</v>
@@ -1267,13 +1265,13 @@
     </row>
     <row r="22" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D22" s="11">
         <v>1</v>
@@ -1288,13 +1286,13 @@
     </row>
     <row r="23" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23" s="11">
         <v>1</v>
@@ -1309,13 +1307,13 @@
     </row>
     <row r="24" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D24" s="11">
         <v>1</v>
@@ -1330,13 +1328,13 @@
     </row>
     <row r="25" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1351,20 +1349,20 @@
     </row>
     <row r="26" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -1377,18 +1375,18 @@
         <v>752</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -1403,13 +1401,13 @@
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1422,18 +1420,18 @@
         <v>65</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -1446,18 +1444,18 @@
         <v>32</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1470,25 +1468,31 @@
         <v>112</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="39">
+        <f>SUM(E28:E31,E19,E9:E12)</f>
+        <v>444</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="25"/>
     </row>
     <row r="34" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D34" s="17">
         <v>2</v>
@@ -1501,18 +1505,18 @@
         <v>20</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D35" s="37">
         <v>3</v>
@@ -1524,18 +1528,18 @@
         <v>0</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D36" s="37">
         <v>2</v>
@@ -1547,18 +1551,18 @@
         <v>0</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D37" s="37">
         <v>3</v>
@@ -1570,18 +1574,18 @@
         <v>0</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="37" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D38" s="37">
         <v>2</v>
@@ -1593,18 +1597,18 @@
         <v>0</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D39" s="9">
         <v>1</v>
@@ -1617,16 +1621,16 @@
         <v>50</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E46" s="27" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F46" s="28">
         <f>SUM(F4:F44)</f>
-        <v>26235</v>
+        <v>26334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated prices and part numbers
</commit_message>
<xml_diff>
--- a/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
+++ b/v4-5-upgrade-2023/v4-5-upgrade-parts-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\v4-5-upgrade-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91A1199-0A66-4DCC-9FE0-9C35FA716CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9458BC8-BCDC-4F0B-9B35-6C3911C5C366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -71,15 +71,9 @@
     <t>Detection: Filter wheel</t>
   </si>
   <si>
-    <t>5-slot filter wheel for 25-mm filters</t>
-  </si>
-  <si>
     <t>ZWO</t>
   </si>
   <si>
-    <t>Check local distributors (astronomy shops)</t>
-  </si>
-  <si>
     <t>3D printed</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>Mitutoyo MT-1 Accessory Tube Lens</t>
   </si>
   <si>
-    <t>Adapter-MitutoyoMT1-SM2.stl</t>
-  </si>
-  <si>
     <t>Adapter for SM2 lens tube, attached to SM2 retaining ring</t>
   </si>
   <si>
@@ -315,6 +306,12 @@
   </si>
   <si>
     <t>Adapter to hold 32 mm filters in 36 mm slots</t>
+  </si>
+  <si>
+    <t>Check local distributors (astronomy shops). Alternative for small (25 mm) filters: 5-slot filter wheel for 25-mm filters</t>
+  </si>
+  <si>
+    <t>Adapter-MitutoyoMT1-SM2-v3(flex).stl</t>
   </si>
 </sst>
 </file>
@@ -583,9 +580,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -623,7 +620,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -729,7 +726,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -871,7 +868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -879,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -911,10 +908,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>4</v>
@@ -980,266 +977,280 @@
       <c r="E6" s="30"/>
       <c r="F6" s="31"/>
     </row>
-    <row r="7" spans="1:8" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>299</v>
+      </c>
+      <c r="F7" s="19">
+        <f>E7*D7</f>
+        <v>299</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>299</v>
-      </c>
-      <c r="F8" s="19">
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>10</v>
+      </c>
+      <c r="F8" s="20">
         <f>E8*D8</f>
-        <v>299</v>
-      </c>
-      <c r="G8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="3">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4">
-        <v>10</v>
-      </c>
-      <c r="F9" s="20">
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>37</v>
+      </c>
+      <c r="F9" s="19">
         <f>E9*D9</f>
-        <v>50</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>91</v>
+        <v>37</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F10" s="19">
         <f>E10*D10</f>
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F11" s="19">
         <f>E11*D11</f>
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>24</v>
-      </c>
-      <c r="F12" s="19">
-        <f>E12*D12</f>
-        <v>48</v>
-      </c>
-      <c r="G12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:8" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
+    </row>
+    <row r="14" spans="1:8" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:8" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-    </row>
-    <row r="16" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4655</v>
+      </c>
+      <c r="F15" s="21">
+        <f>D15*E15</f>
+        <v>4655</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8">
-        <v>4655</v>
-      </c>
-      <c r="F16" s="21">
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10">
+        <v>75</v>
+      </c>
+      <c r="F16" s="22">
         <f>D16*E16</f>
-        <v>4655</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>30</v>
+        <v>75</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
       </c>
       <c r="E17" s="10">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="F17" s="22">
         <f>D17*E17</f>
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="G17" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>200</v>
+      </c>
+      <c r="F18" s="23">
+        <f>D18*E18</f>
+        <v>200</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>26</v>
+      </c>
+      <c r="F19" s="19">
+        <f>E19*D19</f>
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="10">
-        <v>1</v>
-      </c>
-      <c r="E18" s="10">
-        <v>136</v>
-      </c>
-      <c r="F18" s="22">
-        <f>D18*E18</f>
-        <v>136</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="16">
-        <v>1</v>
-      </c>
-      <c r="E19" s="16">
-        <v>100</v>
-      </c>
-      <c r="F19" s="23">
-        <f>D19*E19</f>
-        <v>100</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>26</v>
-      </c>
-      <c r="F20" s="19">
-        <f>E20*D20</f>
-        <v>26</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>62</v>
+      <c r="D20" s="11">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
+        <v>801</v>
+      </c>
+      <c r="F20" s="24">
+        <f>D20*E20</f>
+        <v>801</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1247,7 +1258,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>33</v>
@@ -1256,11 +1267,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="11">
-        <v>801</v>
+        <v>718</v>
       </c>
       <c r="F21" s="24">
-        <f>D21*E21</f>
-        <v>801</v>
+        <f t="shared" ref="F21:F24" si="0">D21*E21</f>
+        <v>718</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1268,7 +1279,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>35</v>
@@ -1277,11 +1288,11 @@
         <v>1</v>
       </c>
       <c r="E22" s="11">
-        <v>718</v>
+        <v>1391</v>
       </c>
       <c r="F22" s="24">
-        <f t="shared" ref="F22:F25" si="0">D22*E22</f>
-        <v>718</v>
+        <f t="shared" si="0"/>
+        <v>1391</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1289,7 +1300,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>37</v>
@@ -1298,105 +1309,108 @@
         <v>1</v>
       </c>
       <c r="E23" s="11">
-        <v>1391</v>
+        <v>883</v>
       </c>
       <c r="F23" s="24">
         <f t="shared" si="0"/>
-        <v>1391</v>
+        <v>883</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="11">
-        <v>1</v>
-      </c>
-      <c r="E24" s="11">
-        <v>883</v>
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3670</v>
       </c>
       <c r="F24" s="24">
         <f t="shared" si="0"/>
-        <v>883</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
         <v>3670</v>
       </c>
-      <c r="F25" s="24">
-        <f t="shared" si="0"/>
-        <v>3670</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    </row>
+    <row r="25" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="25"/>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>752</v>
+      </c>
+      <c r="F26" s="19">
+        <f t="shared" ref="F26:F30" si="1">D26*E26</f>
+        <v>752</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>50</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>752</v>
-      </c>
-      <c r="F27" s="19">
-        <f t="shared" ref="F27:F31" si="1">D27*E27</f>
-        <v>752</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>65</v>
+      </c>
+      <c r="F28" s="19">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D28" s="3">
-        <v>1</v>
-      </c>
-      <c r="E28" s="4">
-        <v>10</v>
-      </c>
-      <c r="F28" s="20">
-        <f t="shared" si="1"/>
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1404,7 +1418,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>48</v>
@@ -1413,11 +1427,11 @@
         <v>1</v>
       </c>
       <c r="E29" s="2">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F29" s="19">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>49</v>
@@ -1428,7 +1442,7 @@
         <v>50</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>51</v>
@@ -1437,207 +1451,183 @@
         <v>1</v>
       </c>
       <c r="E30" s="2">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="F30" s="19">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2">
-        <v>112</v>
-      </c>
-      <c r="F31" s="19">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="39">
-        <f>SUM(E28:E31,E19,E9:E12)</f>
-        <v>444</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="25"/>
-    </row>
-    <row r="34" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="17">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="39">
+        <f>SUM(E27:E30,E18,E8:E11)</f>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="17">
         <v>2</v>
       </c>
-      <c r="E34" s="17">
-        <v>10</v>
-      </c>
-      <c r="F34" s="26">
-        <f>D34*E34</f>
-        <v>20</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>68</v>
+      <c r="E33" s="17">
+        <v>50</v>
+      </c>
+      <c r="F33" s="26">
+        <f>D33*E33</f>
+        <v>100</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="37">
+        <v>3</v>
+      </c>
+      <c r="E34" s="37">
+        <v>150</v>
+      </c>
+      <c r="F34" s="38">
+        <v>0</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>75</v>
-      </c>
       <c r="D35" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35" s="37">
-        <v>150</v>
+        <v>53</v>
       </c>
       <c r="F35" s="38">
         <v>0</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="37" t="s">
-        <v>77</v>
-      </c>
       <c r="D36" s="37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E36" s="37">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="F36" s="38">
         <v>0</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D37" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" s="37">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="F37" s="38">
         <v>0</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" s="37">
-        <v>2</v>
-      </c>
-      <c r="E38" s="37">
         <v>77</v>
       </c>
-      <c r="F38" s="38">
-        <v>0</v>
-      </c>
-      <c r="G38" s="37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="9" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <v>50</v>
+      </c>
+      <c r="F38" s="18">
+        <f>D38*E38</f>
+        <v>50</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E45" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="9">
-        <v>1</v>
-      </c>
-      <c r="E39" s="9">
-        <v>50</v>
-      </c>
-      <c r="F39" s="18">
-        <f>D39*E39</f>
-        <v>50</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E46" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" s="28">
-        <f>SUM(F4:F44)</f>
-        <v>26334</v>
+      <c r="F45" s="28">
+        <f>SUM(F4:F43)</f>
+        <v>26554</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C25" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C27" r:id="rId3" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C26" r:id="rId3" display="MT-1 Accessory Tube Lens" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>